<commit_message>
Use Relative Path To CSV Data For Data Driven Create JMX File.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/create_jmx_files/DataDrivenCreateJMXFile.xlsx
+++ b/src/test/resources/data/create_jmx_files/DataDrivenCreateJMXFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5030FD53-5E4B-4816-9712-4ED745E8C7F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{5030FD53-5E4B-4816-9712-4ED745E8C7F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{21C782E3-2692-4679-8AF7-24D471FA0831}"/>
   <bookViews>
     <workbookView xWindow="-3375" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="134">
   <si>
     <t>Test Plan Name</t>
   </si>
@@ -228,9 +228,6 @@
       &lt;/gsd:gensrv_getpolicydetail&gt;
    &lt;/soap:Body&gt;
 &lt;/soap:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>C:/Users/F5255309/OneDrive - FRG/Downloads/ReactivationUcns.csv</t>
   </si>
   <si>
     <t>policyNo</t>
@@ -698,6 +695,15 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>src/test/resources/data/create_jmx_files/csv_data/data_driven_create_jmx_file.csv</t>
+  </si>
+  <si>
+    <t>Test Plan One</t>
+  </si>
+  <si>
+    <t>Test Plan Two</t>
   </si>
 </sst>
 </file>
@@ -1106,16 +1112,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1128,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,22 +1190,22 @@
         <v>13</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>1</v>
@@ -1276,7 +1282,7 @@
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -1297,18 +1303,18 @@
         <v>5</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N2" t="s">
         <v>15</v>
@@ -1320,13 +1326,13 @@
         <v>17</v>
       </c>
       <c r="Q2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R2" t="s">
         <v>19</v>
       </c>
       <c r="S2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>63</v>
@@ -1338,7 +1344,7 @@
         <v>59</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z2" s="5" t="s">
         <v>61</v>
@@ -1350,10 +1356,10 @@
         <v>1</v>
       </c>
       <c r="AC2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE2" t="s">
         <v>64</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>65</v>
       </c>
       <c r="AF2" t="b">
         <v>0</v>
@@ -1376,7 +1382,7 @@
     </row>
     <row r="3" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -1397,18 +1403,18 @@
         <v>5</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N3" t="s">
         <v>15</v>
@@ -1420,7 +1426,7 @@
         <v>17</v>
       </c>
       <c r="Q3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R3" t="s">
         <v>19</v>
@@ -1429,7 +1435,7 @@
         <v>62</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W3" s="5" t="s">
         <v>58</v>
@@ -1438,7 +1444,7 @@
         <v>60</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>61</v>
@@ -1450,10 +1456,10 @@
         <v>1</v>
       </c>
       <c r="AC3" t="s">
+        <v>131</v>
+      </c>
+      <c r="AE3" t="s">
         <v>64</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>65</v>
       </c>
       <c r="AF3" t="b">
         <v>0</v>
@@ -1520,357 +1526,357 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="G6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="G11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="G13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>

</xml_diff>